<commit_message>
Create web mvc project use spring framework
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sharecare-training\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sharecare-trainning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Report</t>
   </si>
@@ -42,6 +45,9 @@
   </si>
   <si>
     <t>Refactoring CRUD service: use annotation, reflection, generic</t>
+  </si>
+  <si>
+    <t>Create web app and read a show a list books on website.</t>
   </si>
 </sst>
 </file>
@@ -84,8 +90,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -360,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,6 +451,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>42146</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Comment for book: complete CommentService
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Report</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Creating a web app to demo Spring MVC and Mongodb</t>
+  </si>
+  <si>
+    <t>Comment for the demo project: Create, update, delete and get comment on service</t>
   </si>
 </sst>
 </file>
@@ -394,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,6 +462,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>42149</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Get list comment and add new comment on client
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Report</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>Comment for the demo project: Create, update, delete and get comment on service</t>
+  </si>
+  <si>
+    <t>26/5/2015</t>
+  </si>
+  <si>
+    <t>Comment for the demo project: Get list comment of a book and add new comment on client</t>
   </si>
 </sst>
 </file>
@@ -397,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,6 +476,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Build CSS from SASS for the demo project
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -53,10 +53,10 @@
     <t>Comment for the demo project: Create, update, delete and get comment on service</t>
   </si>
   <si>
-    <t>26/5/2015</t>
-  </si>
-  <si>
     <t>Comment for the demo project: Get list comment of a book and add new comment on client</t>
+  </si>
+  <si>
+    <t>Learn SASS and use SASS to create CSS for the demo project</t>
   </si>
 </sst>
 </file>
@@ -403,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,10 +477,18 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1">
+        <v>42150</v>
+      </c>
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>42151</v>
+      </c>
+      <c r="B11" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Authentication use Spring Security
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Report</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Learn SASS and use SASS to create CSS for the demo project</t>
+  </si>
+  <si>
+    <t>Learn Requirejs, Demo project: load more comment, delete comment</t>
+  </si>
+  <si>
+    <t>Spring Security (the demo project has CSRF error in delete comment feature)</t>
   </si>
 </sst>
 </file>
@@ -403,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,6 +498,22 @@
         <v>9</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>42152</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>42153</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Creating mini demo blossom and updating report
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Report</t>
   </si>
@@ -63,6 +63,18 @@
   </si>
   <si>
     <t>Spring Security (the demo project has CSRF error in delete comment feature)</t>
+  </si>
+  <si>
+    <t>Fixing CSRF bug of demo project and Learning Magnolia CMS</t>
+  </si>
+  <si>
+    <t>Magnolia Blossom</t>
+  </si>
+  <si>
+    <t>Received Sharecare project and set up development environment. (A. Nguyen supported me)</t>
+  </si>
+  <si>
+    <t>Learn the structure of Sharecare project.</t>
   </si>
 </sst>
 </file>
@@ -409,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,6 +526,46 @@
         <v>11</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>42156</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>42157</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>42158</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>42159</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>42160</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update report from 6-8 to 6-12
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Report</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>Learn the structure of Sharecare project.</t>
+  </si>
+  <si>
+    <t>Learn Solr and  the structure of Sharecare project.</t>
+  </si>
+  <si>
+    <t>Fix bug: Published question without an answer gives an OOPS page.</t>
+  </si>
+  <si>
+    <t>Write unit test after fix the bug.</t>
   </si>
 </sst>
 </file>
@@ -421,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,6 +575,46 @@
         <v>15</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>42163</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>42164</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>42165</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>42166</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>42167</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update report and create demo-gulp
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Report</t>
   </si>
@@ -84,6 +84,18 @@
   </si>
   <si>
     <t>Write unit test after fix the bug.</t>
+  </si>
+  <si>
+    <t>Learn Gulp tool</t>
+  </si>
+  <si>
+    <t>Learn fixing bug: MAINT-3202</t>
+  </si>
+  <si>
+    <t>Learn fixing bug: MAINT-3222</t>
+  </si>
+  <si>
+    <t>Learn fixing bug: MAINT-3222 and MAINT-3205</t>
   </si>
 </sst>
 </file>
@@ -430,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,6 +627,46 @@
         <v>18</v>
       </c>
     </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>42170</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>42171</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>42172</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>42173</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>42174</v>
+      </c>
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>